<commit_message>
added bars to Gantt Chart
</commit_message>
<xml_diff>
--- a/management/GanttChart_Project.xlsx
+++ b/management/GanttChart_Project.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSC4992Project\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969E0EC1-1D75-48FB-AE04-34AE12C4FD70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Chart" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="64">
   <si>
     <t>GANTT CHART TEMPLATE</t>
   </si>
@@ -47,36 +48,6 @@
   </si>
   <si>
     <t>PERCENT COMPLETE</t>
-  </si>
-  <si>
-    <t>WEEK 1</t>
-  </si>
-  <si>
-    <t>WEEK 2</t>
-  </si>
-  <si>
-    <t>WEEK 3</t>
-  </si>
-  <si>
-    <t>WEEK 4</t>
-  </si>
-  <si>
-    <t>WEEK 5</t>
-  </si>
-  <si>
-    <t>WEEK 6</t>
-  </si>
-  <si>
-    <t>WEEK 7</t>
-  </si>
-  <si>
-    <t>WEEK 8</t>
-  </si>
-  <si>
-    <t>WEEK 9</t>
-  </si>
-  <si>
-    <t>WEEK 10</t>
   </si>
   <si>
     <t>WEEK 11</t>
@@ -175,22 +146,10 @@
     <t>Ibrahim</t>
   </si>
   <si>
-    <t>Create buttons</t>
-  </si>
-  <si>
-    <t>Irbahim</t>
-  </si>
-  <si>
     <t>Project Presentation Practice</t>
   </si>
   <si>
     <t>Start writing presentation slides</t>
-  </si>
-  <si>
-    <t>Add code to documents stats</t>
-  </si>
-  <si>
-    <t>Add display functions for stats</t>
   </si>
   <si>
     <t>Add highscore database</t>
@@ -213,11 +172,59 @@
   <si>
     <t>Proof read presentation slides</t>
   </si>
+  <si>
+    <t>LEVEL</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>Create button images</t>
+  </si>
+  <si>
+    <t>advanced</t>
+  </si>
+  <si>
+    <t>Add code to document statistics</t>
+  </si>
+  <si>
+    <t>Add statistic graphs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/18-2/22 </t>
+  </si>
+  <si>
+    <t>2/25-3/1</t>
+  </si>
+  <si>
+    <t>3/4-3/8</t>
+  </si>
+  <si>
+    <t>3/11-3/15</t>
+  </si>
+  <si>
+    <t>3/18-3/22</t>
+  </si>
+  <si>
+    <t>3/25-3/29</t>
+  </si>
+  <si>
+    <t>4/1-4/5</t>
+  </si>
+  <si>
+    <t>4/8-4/12</t>
+  </si>
+  <si>
+    <t>4/15-4/19</t>
+  </si>
+  <si>
+    <t>4/22-4/26</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d"/>
@@ -280,7 +287,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,12 +375,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor rgb="FF5CBCD6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
@@ -391,8 +392,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="4"/>
         <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FF5CBCD6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,27 +621,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -644,13 +647,40 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,41 +994,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO998"/>
+  <dimension ref="A1:BP998"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="AV33" sqref="AV33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="67" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20" style="46" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="68" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="15.75" customHeight="1">
+    <row r="1" spans="1:68" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
+      <c r="O1" s="1"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -1051,23 +1082,24 @@
       <c r="BM1" s="2"/>
       <c r="BN1" s="2"/>
       <c r="BO1" s="2"/>
-    </row>
-    <row r="2" spans="1:67" ht="15.75" customHeight="1">
+      <c r="BP1" s="2"/>
+    </row>
+    <row r="2" spans="1:68" ht="15.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="1"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1120,25 +1152,26 @@
       <c r="BM2" s="2"/>
       <c r="BN2" s="2"/>
       <c r="BO2" s="2"/>
-    </row>
-    <row r="3" spans="1:67" ht="30" customHeight="1">
-      <c r="A3" s="50" t="s">
+      <c r="BP2" s="2"/>
+    </row>
+    <row r="3" spans="1:68" ht="30" customHeight="1">
+      <c r="A3" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="7"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -1155,14 +1188,14 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="5"/>
+      <c r="AF3" s="7"/>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
-      <c r="AM3" s="8"/>
+      <c r="AM3" s="5"/>
       <c r="AN3" s="8"/>
       <c r="AO3" s="8"/>
       <c r="AP3" s="8"/>
@@ -1191,8 +1224,9 @@
       <c r="BM3" s="8"/>
       <c r="BN3" s="8"/>
       <c r="BO3" s="8"/>
-    </row>
-    <row r="4" spans="1:67" ht="15.75" customHeight="1">
+      <c r="BP3" s="8"/>
+    </row>
+    <row r="4" spans="1:68" ht="15.75" customHeight="1">
       <c r="A4" s="9"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1205,7 +1239,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="1"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -1260,8 +1294,9 @@
       <c r="BM4" s="2"/>
       <c r="BN4" s="2"/>
       <c r="BO4" s="2"/>
-    </row>
-    <row r="5" spans="1:67" ht="15.75" customHeight="1">
+      <c r="BP4" s="2"/>
+    </row>
+    <row r="5" spans="1:68" ht="15.75" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1274,7 +1309,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -1329,316 +1364,321 @@
       <c r="BM5" s="2"/>
       <c r="BN5" s="2"/>
       <c r="BO5" s="2"/>
-    </row>
-    <row r="6" spans="1:67" ht="15">
-      <c r="A6" s="48"/>
-      <c r="B6" s="48" t="s">
+      <c r="BP5" s="2"/>
+    </row>
+    <row r="6" spans="1:68" ht="15">
+      <c r="A6" s="73"/>
+      <c r="B6" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="E6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="F6" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="G6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="H6" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="I6" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
+      <c r="X6" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="71"/>
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD6" s="71"/>
+      <c r="AE6" s="71"/>
+      <c r="AF6" s="71"/>
+      <c r="AG6" s="71"/>
+      <c r="AH6" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI6" s="71"/>
+      <c r="AJ6" s="71"/>
+      <c r="AK6" s="71"/>
+      <c r="AL6" s="71"/>
+      <c r="AM6" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN6" s="71"/>
+      <c r="AO6" s="71"/>
+      <c r="AP6" s="71"/>
+      <c r="AQ6" s="71"/>
+      <c r="AR6" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS6" s="71"/>
+      <c r="AT6" s="71"/>
+      <c r="AU6" s="71"/>
+      <c r="AV6" s="71"/>
+      <c r="AW6" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX6" s="71"/>
+      <c r="AY6" s="71"/>
+      <c r="AZ6" s="71"/>
+      <c r="BA6" s="71"/>
+      <c r="BB6" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC6" s="71"/>
+      <c r="BD6" s="71"/>
+      <c r="BE6" s="71"/>
+      <c r="BF6" s="71"/>
+      <c r="BG6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="46" t="s">
+      <c r="BH6" s="71"/>
+      <c r="BI6" s="71"/>
+      <c r="BJ6" s="71"/>
+      <c r="BK6" s="71"/>
+      <c r="BL6" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="54" t="s">
+      <c r="BM6" s="71"/>
+      <c r="BN6" s="71"/>
+      <c r="BO6" s="71"/>
+      <c r="BP6" s="71"/>
+    </row>
+    <row r="7" spans="1:68" ht="15">
+      <c r="A7" s="74"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="46" t="s">
+      <c r="J7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="47"/>
-      <c r="Z6" s="47"/>
-      <c r="AA6" s="47"/>
-      <c r="AB6" s="54" t="s">
+      <c r="K7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AC6" s="47"/>
-      <c r="AD6" s="47"/>
-      <c r="AE6" s="47"/>
-      <c r="AF6" s="47"/>
-      <c r="AG6" s="46" t="s">
+      <c r="L7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AH6" s="47"/>
-      <c r="AI6" s="47"/>
-      <c r="AJ6" s="47"/>
-      <c r="AK6" s="47"/>
-      <c r="AL6" s="54" t="s">
+      <c r="M7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AM6" s="47"/>
-      <c r="AN6" s="47"/>
-      <c r="AO6" s="47"/>
-      <c r="AP6" s="47"/>
-      <c r="AQ6" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
-      <c r="AT6" s="47"/>
-      <c r="AU6" s="47"/>
-      <c r="AV6" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW6" s="47"/>
-      <c r="AX6" s="47"/>
-      <c r="AY6" s="47"/>
-      <c r="AZ6" s="47"/>
-      <c r="BA6" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB6" s="47"/>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="47"/>
-      <c r="BE6" s="47"/>
-      <c r="BF6" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="BG6" s="47"/>
-      <c r="BH6" s="47"/>
-      <c r="BI6" s="47"/>
-      <c r="BJ6" s="47"/>
-      <c r="BK6" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="BL6" s="47"/>
-      <c r="BM6" s="47"/>
-      <c r="BN6" s="47"/>
-      <c r="BO6" s="47"/>
-    </row>
-    <row r="7" spans="1:67" ht="15">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>19</v>
-      </c>
       <c r="N7" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="V7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="W7" s="12" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="X7" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB7" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="AC7" s="10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AD7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG7" s="12" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="AH7" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AI7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL7" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL7" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="AM7" s="10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AN7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AQ7" s="12" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="AO7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ7" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="AR7" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AS7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV7" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="AT7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV7" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="AW7" s="10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AX7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BA7" s="12" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="AY7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA7" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="BB7" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="BC7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="BD7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="BE7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BF7" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="BD7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="BE7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="BF7" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="BG7" s="10" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="BH7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="BI7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="BJ7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BK7" s="12" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="BI7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="BJ7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK7" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="BL7" s="12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="BM7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="BN7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="BO7" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:67">
+        <v>10</v>
+      </c>
+      <c r="BN7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="BO7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="BP7" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:68">
       <c r="A8" s="14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="16"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
@@ -1694,585 +1734,608 @@
       <c r="BM8" s="16"/>
       <c r="BN8" s="16"/>
       <c r="BO8" s="16"/>
-    </row>
-    <row r="9" spans="1:67" ht="15">
+      <c r="BP8" s="16"/>
+    </row>
+    <row r="9" spans="1:68" ht="15">
       <c r="B9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="20">
+        <v>14</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="20">
         <v>43515</v>
       </c>
-      <c r="D9" s="20">
+      <c r="E9" s="20">
         <v>43517</v>
       </c>
-      <c r="E9" s="21">
-        <f>NETWORKDAYS(C9,D9)</f>
+      <c r="F9" s="21">
+        <f>NETWORKDAYS(D9,E9)</f>
         <v>3</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="22">
+      <c r="G9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="22">
         <v>1</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="26"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="26"/>
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
-      <c r="R9" s="25"/>
+      <c r="R9" s="26"/>
       <c r="S9" s="25"/>
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
       <c r="V9" s="25"/>
-      <c r="W9" s="26"/>
+      <c r="W9" s="25"/>
       <c r="X9" s="26"/>
       <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
       <c r="AA9" s="26"/>
-      <c r="AB9" s="27"/>
+      <c r="AB9" s="26"/>
       <c r="AC9" s="27"/>
       <c r="AD9" s="27"/>
       <c r="AE9" s="27"/>
       <c r="AF9" s="27"/>
-      <c r="AG9" s="26"/>
+      <c r="AG9" s="27"/>
       <c r="AH9" s="26"/>
       <c r="AI9" s="26"/>
       <c r="AJ9" s="26"/>
       <c r="AK9" s="26"/>
-      <c r="AL9" s="27"/>
+      <c r="AL9" s="26"/>
       <c r="AM9" s="27"/>
       <c r="AN9" s="27"/>
       <c r="AO9" s="27"/>
       <c r="AP9" s="27"/>
-      <c r="AQ9" s="26"/>
+      <c r="AQ9" s="27"/>
       <c r="AR9" s="26"/>
       <c r="AS9" s="26"/>
       <c r="AT9" s="26"/>
       <c r="AU9" s="26"/>
-      <c r="AV9" s="25"/>
+      <c r="AV9" s="26"/>
       <c r="AW9" s="25"/>
       <c r="AX9" s="25"/>
       <c r="AY9" s="25"/>
       <c r="AZ9" s="25"/>
-      <c r="BA9" s="26"/>
+      <c r="BA9" s="25"/>
       <c r="BB9" s="26"/>
       <c r="BC9" s="26"/>
       <c r="BD9" s="26"/>
       <c r="BE9" s="26"/>
-      <c r="BF9" s="27"/>
+      <c r="BF9" s="26"/>
       <c r="BG9" s="27"/>
       <c r="BH9" s="27"/>
       <c r="BI9" s="27"/>
       <c r="BJ9" s="27"/>
-      <c r="BK9" s="26"/>
+      <c r="BK9" s="27"/>
       <c r="BL9" s="26"/>
       <c r="BM9" s="26"/>
       <c r="BN9" s="26"/>
-      <c r="BO9" s="28"/>
-    </row>
-    <row r="10" spans="1:67" ht="30">
+      <c r="BO9" s="26"/>
+      <c r="BP9" s="28"/>
+    </row>
+    <row r="10" spans="1:68" ht="30">
       <c r="B10" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="20">
+        <v>16</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="20">
         <v>43515</v>
       </c>
-      <c r="D10" s="20">
+      <c r="E10" s="20">
         <v>43522</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="29">
+      <c r="F10" s="21"/>
+      <c r="G10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="29">
         <v>0.7</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="26"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
-      <c r="R10" s="25"/>
+      <c r="R10" s="26"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-      <c r="W10" s="26"/>
+      <c r="W10" s="25"/>
       <c r="X10" s="26"/>
       <c r="Y10" s="26"/>
       <c r="Z10" s="26"/>
       <c r="AA10" s="26"/>
-      <c r="AB10" s="27"/>
+      <c r="AB10" s="26"/>
       <c r="AC10" s="27"/>
       <c r="AD10" s="27"/>
       <c r="AE10" s="27"/>
       <c r="AF10" s="27"/>
-      <c r="AG10" s="26"/>
+      <c r="AG10" s="27"/>
       <c r="AH10" s="26"/>
       <c r="AI10" s="26"/>
       <c r="AJ10" s="26"/>
       <c r="AK10" s="26"/>
-      <c r="AL10" s="27"/>
+      <c r="AL10" s="26"/>
       <c r="AM10" s="27"/>
       <c r="AN10" s="27"/>
       <c r="AO10" s="27"/>
       <c r="AP10" s="27"/>
-      <c r="AQ10" s="26"/>
+      <c r="AQ10" s="27"/>
       <c r="AR10" s="26"/>
       <c r="AS10" s="26"/>
       <c r="AT10" s="26"/>
       <c r="AU10" s="26"/>
-      <c r="AV10" s="25"/>
+      <c r="AV10" s="26"/>
       <c r="AW10" s="25"/>
       <c r="AX10" s="25"/>
       <c r="AY10" s="25"/>
       <c r="AZ10" s="25"/>
-      <c r="BA10" s="26"/>
+      <c r="BA10" s="25"/>
       <c r="BB10" s="26"/>
       <c r="BC10" s="26"/>
       <c r="BD10" s="26"/>
       <c r="BE10" s="26"/>
-      <c r="BF10" s="27"/>
+      <c r="BF10" s="26"/>
       <c r="BG10" s="27"/>
       <c r="BH10" s="27"/>
       <c r="BI10" s="27"/>
       <c r="BJ10" s="27"/>
-      <c r="BK10" s="26"/>
+      <c r="BK10" s="27"/>
       <c r="BL10" s="26"/>
       <c r="BM10" s="26"/>
       <c r="BN10" s="26"/>
-      <c r="BO10" s="28"/>
-    </row>
-    <row r="11" spans="1:67" ht="15">
+      <c r="BO10" s="26"/>
+      <c r="BP10" s="28"/>
+    </row>
+    <row r="11" spans="1:68" ht="15">
       <c r="B11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="20">
+        <v>18</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="20">
         <v>43515</v>
       </c>
-      <c r="D11" s="20">
+      <c r="E11" s="20">
         <v>43536</v>
       </c>
-      <c r="E11" s="21">
-        <f t="shared" ref="E11:E15" si="0">NETWORKDAYS(C11,D11)</f>
+      <c r="F11" s="21">
+        <f t="shared" ref="F11:F15" si="0">NETWORKDAYS(D11,E11)</f>
         <v>16</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="22">
+      <c r="G11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="22">
         <v>0.2</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="82"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="82"/>
+      <c r="Y11" s="82"/>
       <c r="Z11" s="26"/>
       <c r="AA11" s="26"/>
-      <c r="AB11" s="27"/>
+      <c r="AB11" s="26"/>
       <c r="AC11" s="27"/>
       <c r="AD11" s="27"/>
       <c r="AE11" s="27"/>
       <c r="AF11" s="27"/>
-      <c r="AG11" s="26"/>
+      <c r="AG11" s="27"/>
       <c r="AH11" s="26"/>
       <c r="AI11" s="26"/>
       <c r="AJ11" s="26"/>
       <c r="AK11" s="26"/>
-      <c r="AL11" s="27"/>
+      <c r="AL11" s="26"/>
       <c r="AM11" s="27"/>
       <c r="AN11" s="27"/>
       <c r="AO11" s="27"/>
       <c r="AP11" s="27"/>
-      <c r="AQ11" s="26"/>
+      <c r="AQ11" s="27"/>
       <c r="AR11" s="26"/>
       <c r="AS11" s="26"/>
       <c r="AT11" s="26"/>
       <c r="AU11" s="26"/>
-      <c r="AV11" s="25"/>
+      <c r="AV11" s="26"/>
       <c r="AW11" s="25"/>
       <c r="AX11" s="25"/>
       <c r="AY11" s="25"/>
       <c r="AZ11" s="25"/>
-      <c r="BA11" s="26"/>
+      <c r="BA11" s="25"/>
       <c r="BB11" s="26"/>
       <c r="BC11" s="26"/>
       <c r="BD11" s="26"/>
       <c r="BE11" s="26"/>
-      <c r="BF11" s="27"/>
+      <c r="BF11" s="26"/>
       <c r="BG11" s="27"/>
       <c r="BH11" s="27"/>
       <c r="BI11" s="27"/>
       <c r="BJ11" s="27"/>
-      <c r="BK11" s="26"/>
+      <c r="BK11" s="27"/>
       <c r="BL11" s="26"/>
       <c r="BM11" s="26"/>
       <c r="BN11" s="26"/>
-      <c r="BO11" s="28"/>
-    </row>
-    <row r="12" spans="1:67" ht="30">
+      <c r="BO11" s="26"/>
+      <c r="BP11" s="28"/>
+    </row>
+    <row r="12" spans="1:68" ht="30">
       <c r="B12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="20">
+        <v>20</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="20">
         <v>43522</v>
       </c>
-      <c r="D12" s="20">
+      <c r="E12" s="20">
         <v>43531</v>
       </c>
-      <c r="E12" s="21">
+      <c r="F12" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="30">
+      <c r="G12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="30">
         <v>0</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="67"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="70"/>
-      <c r="V12" s="70"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="81"/>
+      <c r="S12" s="81"/>
+      <c r="T12" s="66"/>
+      <c r="U12" s="66"/>
+      <c r="V12" s="66"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
       <c r="Z12" s="26"/>
       <c r="AA12" s="26"/>
-      <c r="AB12" s="27"/>
+      <c r="AB12" s="26"/>
       <c r="AC12" s="27"/>
       <c r="AD12" s="27"/>
       <c r="AE12" s="27"/>
       <c r="AF12" s="27"/>
-      <c r="AG12" s="26"/>
+      <c r="AG12" s="27"/>
       <c r="AH12" s="26"/>
       <c r="AI12" s="26"/>
       <c r="AJ12" s="26"/>
       <c r="AK12" s="26"/>
-      <c r="AL12" s="27"/>
+      <c r="AL12" s="26"/>
       <c r="AM12" s="27"/>
       <c r="AN12" s="27"/>
       <c r="AO12" s="27"/>
       <c r="AP12" s="27"/>
-      <c r="AQ12" s="26"/>
+      <c r="AQ12" s="27"/>
       <c r="AR12" s="26"/>
       <c r="AS12" s="26"/>
       <c r="AT12" s="26"/>
       <c r="AU12" s="26"/>
-      <c r="AV12" s="25"/>
+      <c r="AV12" s="26"/>
       <c r="AW12" s="25"/>
       <c r="AX12" s="25"/>
       <c r="AY12" s="25"/>
       <c r="AZ12" s="25"/>
-      <c r="BA12" s="26"/>
+      <c r="BA12" s="25"/>
       <c r="BB12" s="26"/>
       <c r="BC12" s="26"/>
       <c r="BD12" s="26"/>
       <c r="BE12" s="26"/>
-      <c r="BF12" s="27"/>
+      <c r="BF12" s="26"/>
       <c r="BG12" s="27"/>
       <c r="BH12" s="27"/>
       <c r="BI12" s="27"/>
       <c r="BJ12" s="27"/>
-      <c r="BK12" s="26"/>
+      <c r="BK12" s="27"/>
       <c r="BL12" s="26"/>
       <c r="BM12" s="26"/>
       <c r="BN12" s="26"/>
-      <c r="BO12" s="28"/>
-    </row>
-    <row r="13" spans="1:67" ht="15">
+      <c r="BO12" s="26"/>
+      <c r="BP12" s="28"/>
+    </row>
+    <row r="13" spans="1:68" ht="15">
       <c r="B13" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="20">
+        <v>22</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="20">
         <v>43522</v>
       </c>
-      <c r="D13" s="20">
+      <c r="E13" s="20">
         <v>43525</v>
       </c>
-      <c r="E13" s="21">
+      <c r="F13" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="31">
+      <c r="G13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="31">
         <v>0.5</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="67"/>
-      <c r="T13" s="67"/>
-      <c r="U13" s="70"/>
-      <c r="V13" s="70"/>
-      <c r="W13" s="26"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="61"/>
+      <c r="W13" s="61"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
       <c r="Z13" s="26"/>
       <c r="AA13" s="26"/>
-      <c r="AB13" s="27"/>
+      <c r="AB13" s="26"/>
       <c r="AC13" s="27"/>
       <c r="AD13" s="27"/>
       <c r="AE13" s="27"/>
       <c r="AF13" s="27"/>
-      <c r="AG13" s="26"/>
+      <c r="AG13" s="27"/>
       <c r="AH13" s="26"/>
       <c r="AI13" s="26"/>
       <c r="AJ13" s="26"/>
       <c r="AK13" s="26"/>
-      <c r="AL13" s="27"/>
+      <c r="AL13" s="26"/>
       <c r="AM13" s="27"/>
       <c r="AN13" s="27"/>
       <c r="AO13" s="27"/>
       <c r="AP13" s="27"/>
-      <c r="AQ13" s="26"/>
+      <c r="AQ13" s="27"/>
       <c r="AR13" s="26"/>
       <c r="AS13" s="26"/>
       <c r="AT13" s="26"/>
       <c r="AU13" s="26"/>
-      <c r="AV13" s="25"/>
+      <c r="AV13" s="26"/>
       <c r="AW13" s="25"/>
       <c r="AX13" s="25"/>
       <c r="AY13" s="25"/>
       <c r="AZ13" s="25"/>
-      <c r="BA13" s="26"/>
+      <c r="BA13" s="25"/>
       <c r="BB13" s="26"/>
       <c r="BC13" s="26"/>
       <c r="BD13" s="26"/>
       <c r="BE13" s="26"/>
-      <c r="BF13" s="27"/>
+      <c r="BF13" s="26"/>
       <c r="BG13" s="27"/>
       <c r="BH13" s="27"/>
       <c r="BI13" s="27"/>
       <c r="BJ13" s="27"/>
-      <c r="BK13" s="26"/>
+      <c r="BK13" s="27"/>
       <c r="BL13" s="26"/>
       <c r="BM13" s="26"/>
       <c r="BN13" s="26"/>
-      <c r="BO13" s="28"/>
-    </row>
-    <row r="14" spans="1:67" ht="15">
+      <c r="BO13" s="26"/>
+      <c r="BP13" s="28"/>
+    </row>
+    <row r="14" spans="1:68" ht="15">
       <c r="B14" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="20">
+        <v>24</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="20">
         <v>43523</v>
       </c>
-      <c r="D14" s="20">
+      <c r="E14" s="20">
         <v>43525</v>
       </c>
-      <c r="E14" s="21">
+      <c r="F14" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="32">
+      <c r="G14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="32">
         <v>0.5</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="69"/>
-      <c r="R14" s="70"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="67"/>
-      <c r="V14" s="70"/>
-      <c r="W14" s="26"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="82"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="61"/>
       <c r="X14" s="26"/>
       <c r="Y14" s="26"/>
       <c r="Z14" s="26"/>
       <c r="AA14" s="26"/>
-      <c r="AB14" s="27"/>
+      <c r="AB14" s="26"/>
       <c r="AC14" s="27"/>
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
       <c r="AF14" s="27"/>
-      <c r="AG14" s="26"/>
+      <c r="AG14" s="27"/>
       <c r="AH14" s="26"/>
       <c r="AI14" s="26"/>
       <c r="AJ14" s="26"/>
       <c r="AK14" s="26"/>
-      <c r="AL14" s="27"/>
+      <c r="AL14" s="26"/>
       <c r="AM14" s="27"/>
       <c r="AN14" s="27"/>
       <c r="AO14" s="27"/>
       <c r="AP14" s="27"/>
-      <c r="AQ14" s="26"/>
+      <c r="AQ14" s="27"/>
       <c r="AR14" s="26"/>
       <c r="AS14" s="26"/>
       <c r="AT14" s="26"/>
       <c r="AU14" s="26"/>
-      <c r="AV14" s="25"/>
+      <c r="AV14" s="26"/>
       <c r="AW14" s="25"/>
       <c r="AX14" s="25"/>
       <c r="AY14" s="25"/>
       <c r="AZ14" s="25"/>
-      <c r="BA14" s="26"/>
+      <c r="BA14" s="25"/>
       <c r="BB14" s="26"/>
       <c r="BC14" s="26"/>
       <c r="BD14" s="26"/>
       <c r="BE14" s="26"/>
-      <c r="BF14" s="27"/>
+      <c r="BF14" s="26"/>
       <c r="BG14" s="27"/>
       <c r="BH14" s="27"/>
       <c r="BI14" s="27"/>
       <c r="BJ14" s="27"/>
-      <c r="BK14" s="26"/>
+      <c r="BK14" s="27"/>
       <c r="BL14" s="26"/>
       <c r="BM14" s="26"/>
       <c r="BN14" s="26"/>
-      <c r="BO14" s="28"/>
-    </row>
-    <row r="15" spans="1:67" s="45" customFormat="1" ht="15">
-      <c r="B15" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="59">
+      <c r="BO14" s="26"/>
+      <c r="BP14" s="28"/>
+    </row>
+    <row r="15" spans="1:68" s="45" customFormat="1" ht="15">
+      <c r="B15" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="51">
         <v>43525</v>
       </c>
-      <c r="D15" s="59">
-        <v>43527</v>
-      </c>
-      <c r="E15" s="60">
+      <c r="E15" s="51">
+        <v>43528</v>
+      </c>
+      <c r="F15" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="61">
+        <v>2</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="53">
         <v>0</v>
       </c>
-      <c r="H15" s="62"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="71"/>
-      <c r="T15" s="72"/>
-      <c r="U15" s="72"/>
-      <c r="V15" s="73"/>
-      <c r="W15" s="65"/>
-      <c r="X15" s="65"/>
-      <c r="Y15" s="65"/>
-      <c r="Z15" s="65"/>
-      <c r="AA15" s="65"/>
-      <c r="AB15" s="66"/>
-      <c r="AC15" s="66"/>
-      <c r="AD15" s="66"/>
-      <c r="AE15" s="66"/>
-      <c r="AF15" s="66"/>
-      <c r="AG15" s="65"/>
-      <c r="AH15" s="65"/>
-      <c r="AI15" s="65"/>
-      <c r="AJ15" s="65"/>
-      <c r="AK15" s="65"/>
-      <c r="AL15" s="66"/>
-      <c r="AM15" s="66"/>
-      <c r="AN15" s="66"/>
-      <c r="AO15" s="66"/>
-      <c r="AP15" s="66"/>
-      <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
-      <c r="AS15" s="65"/>
-      <c r="AT15" s="65"/>
-      <c r="AU15" s="65"/>
-      <c r="AV15" s="64"/>
-      <c r="AW15" s="64"/>
-      <c r="AX15" s="64"/>
-      <c r="AY15" s="64"/>
-      <c r="AZ15" s="64"/>
-      <c r="BA15" s="65"/>
-      <c r="BB15" s="65"/>
-      <c r="BC15" s="65"/>
-      <c r="BD15" s="65"/>
-      <c r="BE15" s="65"/>
-      <c r="BF15" s="66"/>
-      <c r="BG15" s="66"/>
-      <c r="BH15" s="66"/>
-      <c r="BI15" s="66"/>
-      <c r="BJ15" s="66"/>
-      <c r="BK15" s="65"/>
-      <c r="BL15" s="65"/>
-      <c r="BM15" s="65"/>
-      <c r="BN15" s="65"/>
-      <c r="BO15" s="65"/>
-    </row>
-    <row r="16" spans="1:67">
+      <c r="I15" s="54"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="84"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="64"/>
+      <c r="X15" s="57"/>
+      <c r="Y15" s="57"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="57"/>
+      <c r="AB15" s="57"/>
+      <c r="AC15" s="58"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="58"/>
+      <c r="AF15" s="58"/>
+      <c r="AG15" s="58"/>
+      <c r="AH15" s="57"/>
+      <c r="AI15" s="57"/>
+      <c r="AJ15" s="57"/>
+      <c r="AK15" s="57"/>
+      <c r="AL15" s="57"/>
+      <c r="AM15" s="58"/>
+      <c r="AN15" s="58"/>
+      <c r="AO15" s="58"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="58"/>
+      <c r="AR15" s="57"/>
+      <c r="AS15" s="57"/>
+      <c r="AT15" s="57"/>
+      <c r="AU15" s="57"/>
+      <c r="AV15" s="57"/>
+      <c r="AW15" s="56"/>
+      <c r="AX15" s="56"/>
+      <c r="AY15" s="56"/>
+      <c r="AZ15" s="56"/>
+      <c r="BA15" s="56"/>
+      <c r="BB15" s="57"/>
+      <c r="BC15" s="57"/>
+      <c r="BD15" s="57"/>
+      <c r="BE15" s="57"/>
+      <c r="BF15" s="57"/>
+      <c r="BG15" s="58"/>
+      <c r="BH15" s="58"/>
+      <c r="BI15" s="58"/>
+      <c r="BJ15" s="58"/>
+      <c r="BK15" s="58"/>
+      <c r="BL15" s="57"/>
+      <c r="BM15" s="57"/>
+      <c r="BN15" s="57"/>
+      <c r="BO15" s="57"/>
+      <c r="BP15" s="57"/>
+    </row>
+    <row r="16" spans="1:68">
       <c r="A16" s="14" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="36"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
       <c r="K16" s="36"/>
-      <c r="L16" s="34"/>
+      <c r="L16" s="36"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
@@ -2328,433 +2391,449 @@
       <c r="BM16" s="34"/>
       <c r="BN16" s="34"/>
       <c r="BO16" s="34"/>
-    </row>
-    <row r="17" spans="1:67" ht="15">
+      <c r="BP16" s="34"/>
+    </row>
+    <row r="17" spans="1:68" ht="15">
       <c r="B17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="37">
+        <v>30</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="37">
         <v>43526</v>
       </c>
-      <c r="D17" s="37">
+      <c r="E17" s="37">
         <v>43530</v>
       </c>
-      <c r="E17" s="21">
-        <f>NETWORKDAYS(C17,D17)</f>
+      <c r="F17" s="21">
+        <f>NETWORKDAYS(D17,E17)</f>
         <v>3</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="38">
+      <c r="G17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="38">
         <v>0</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="25"/>
       <c r="L17" s="25"/>
-      <c r="M17" s="26"/>
+      <c r="M17" s="25"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="25"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
+      <c r="U17" s="66"/>
       <c r="V17" s="25"/>
-      <c r="W17" s="26"/>
+      <c r="W17" s="25"/>
       <c r="X17" s="26"/>
       <c r="Y17" s="26"/>
       <c r="Z17" s="26"/>
       <c r="AA17" s="26"/>
-      <c r="AB17" s="27"/>
+      <c r="AB17" s="26"/>
       <c r="AC17" s="27"/>
       <c r="AD17" s="27"/>
       <c r="AE17" s="27"/>
       <c r="AF17" s="27"/>
-      <c r="AG17" s="26"/>
+      <c r="AG17" s="27"/>
       <c r="AH17" s="26"/>
       <c r="AI17" s="26"/>
       <c r="AJ17" s="26"/>
       <c r="AK17" s="26"/>
-      <c r="AL17" s="27"/>
+      <c r="AL17" s="26"/>
       <c r="AM17" s="27"/>
       <c r="AN17" s="27"/>
       <c r="AO17" s="27"/>
       <c r="AP17" s="27"/>
-      <c r="AQ17" s="26"/>
+      <c r="AQ17" s="27"/>
       <c r="AR17" s="26"/>
       <c r="AS17" s="26"/>
       <c r="AT17" s="26"/>
       <c r="AU17" s="26"/>
-      <c r="AV17" s="25"/>
+      <c r="AV17" s="26"/>
       <c r="AW17" s="25"/>
       <c r="AX17" s="25"/>
       <c r="AY17" s="25"/>
       <c r="AZ17" s="25"/>
-      <c r="BA17" s="26"/>
+      <c r="BA17" s="25"/>
       <c r="BB17" s="26"/>
       <c r="BC17" s="26"/>
       <c r="BD17" s="26"/>
       <c r="BE17" s="26"/>
-      <c r="BF17" s="27"/>
+      <c r="BF17" s="26"/>
       <c r="BG17" s="27"/>
       <c r="BH17" s="27"/>
       <c r="BI17" s="27"/>
       <c r="BJ17" s="27"/>
-      <c r="BK17" s="26"/>
+      <c r="BK17" s="27"/>
       <c r="BL17" s="26"/>
       <c r="BM17" s="26"/>
       <c r="BN17" s="26"/>
-      <c r="BO17" s="28"/>
-    </row>
-    <row r="18" spans="1:67" s="45" customFormat="1" ht="15">
+      <c r="BO17" s="26"/>
+      <c r="BP17" s="28"/>
+    </row>
+    <row r="18" spans="1:68" s="45" customFormat="1" ht="15">
       <c r="B18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="37">
+      <c r="D18" s="37">
         <v>43526</v>
       </c>
-      <c r="D18" s="37">
+      <c r="E18" s="37">
         <v>43529</v>
       </c>
-      <c r="E18" s="21">
-        <f>NETWORKDAYS(C18,D18)</f>
+      <c r="F18" s="21">
+        <f>NETWORKDAYS(D18,E18)</f>
         <v>2</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="38">
+      <c r="G18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="38">
         <v>0</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
-      <c r="M18" s="26"/>
+      <c r="M18" s="25"/>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
       <c r="U18" s="25"/>
       <c r="V18" s="25"/>
-      <c r="W18" s="26"/>
+      <c r="W18" s="25"/>
       <c r="X18" s="26"/>
       <c r="Y18" s="26"/>
       <c r="Z18" s="26"/>
       <c r="AA18" s="26"/>
-      <c r="AB18" s="27"/>
+      <c r="AB18" s="26"/>
       <c r="AC18" s="27"/>
       <c r="AD18" s="27"/>
       <c r="AE18" s="27"/>
       <c r="AF18" s="27"/>
-      <c r="AG18" s="26"/>
+      <c r="AG18" s="27"/>
       <c r="AH18" s="26"/>
       <c r="AI18" s="26"/>
       <c r="AJ18" s="26"/>
       <c r="AK18" s="26"/>
-      <c r="AL18" s="27"/>
+      <c r="AL18" s="26"/>
       <c r="AM18" s="27"/>
       <c r="AN18" s="27"/>
       <c r="AO18" s="27"/>
       <c r="AP18" s="27"/>
-      <c r="AQ18" s="26"/>
+      <c r="AQ18" s="27"/>
       <c r="AR18" s="26"/>
       <c r="AS18" s="26"/>
       <c r="AT18" s="26"/>
       <c r="AU18" s="26"/>
-      <c r="AV18" s="25"/>
+      <c r="AV18" s="26"/>
       <c r="AW18" s="25"/>
       <c r="AX18" s="25"/>
       <c r="AY18" s="25"/>
       <c r="AZ18" s="25"/>
-      <c r="BA18" s="26"/>
+      <c r="BA18" s="25"/>
       <c r="BB18" s="26"/>
       <c r="BC18" s="26"/>
       <c r="BD18" s="26"/>
       <c r="BE18" s="26"/>
-      <c r="BF18" s="27"/>
+      <c r="BF18" s="26"/>
       <c r="BG18" s="27"/>
       <c r="BH18" s="27"/>
       <c r="BI18" s="27"/>
       <c r="BJ18" s="27"/>
-      <c r="BK18" s="26"/>
+      <c r="BK18" s="27"/>
       <c r="BL18" s="26"/>
       <c r="BM18" s="26"/>
       <c r="BN18" s="26"/>
-      <c r="BO18" s="28"/>
-    </row>
-    <row r="19" spans="1:67" ht="15">
+      <c r="BO18" s="26"/>
+      <c r="BP18" s="28"/>
+    </row>
+    <row r="19" spans="1:68" ht="15">
       <c r="B19" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="37">
+        <v>29</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="37">
         <v>43529</v>
       </c>
-      <c r="D19" s="37">
+      <c r="E19" s="37">
         <v>43552</v>
       </c>
-      <c r="E19" s="21">
-        <f t="shared" ref="E19:E21" si="1">NETWORKDAYS(C19,D19)</f>
+      <c r="F19" s="21">
+        <f t="shared" ref="F19:F21" si="1">NETWORKDAYS(D19,E19)</f>
         <v>18</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="39">
+      <c r="G19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="39">
         <v>0</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
-      <c r="M19" s="26"/>
+      <c r="M19" s="25"/>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
       <c r="Q19" s="26"/>
-      <c r="R19" s="25"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="25"/>
-      <c r="T19" s="25"/>
-      <c r="U19" s="25"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="27"/>
-      <c r="AC19" s="27"/>
-      <c r="AD19" s="27"/>
-      <c r="AE19" s="27"/>
-      <c r="AF19" s="27"/>
-      <c r="AG19" s="26"/>
-      <c r="AH19" s="26"/>
-      <c r="AI19" s="26"/>
-      <c r="AJ19" s="26"/>
-      <c r="AK19" s="26"/>
-      <c r="AL19" s="27"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="66"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="66"/>
+      <c r="X19" s="82"/>
+      <c r="Y19" s="82"/>
+      <c r="Z19" s="82"/>
+      <c r="AA19" s="82"/>
+      <c r="AB19" s="82"/>
+      <c r="AC19" s="85"/>
+      <c r="AD19" s="85"/>
+      <c r="AE19" s="85"/>
+      <c r="AF19" s="85"/>
+      <c r="AG19" s="85"/>
+      <c r="AH19" s="82"/>
+      <c r="AI19" s="82"/>
+      <c r="AJ19" s="82"/>
+      <c r="AK19" s="82"/>
+      <c r="AL19" s="26"/>
       <c r="AM19" s="27"/>
       <c r="AN19" s="27"/>
       <c r="AO19" s="27"/>
       <c r="AP19" s="27"/>
-      <c r="AQ19" s="26"/>
+      <c r="AQ19" s="27"/>
       <c r="AR19" s="26"/>
       <c r="AS19" s="26"/>
       <c r="AT19" s="26"/>
       <c r="AU19" s="26"/>
-      <c r="AV19" s="25"/>
+      <c r="AV19" s="26"/>
       <c r="AW19" s="25"/>
       <c r="AX19" s="25"/>
       <c r="AY19" s="25"/>
       <c r="AZ19" s="25"/>
-      <c r="BA19" s="26"/>
+      <c r="BA19" s="25"/>
       <c r="BB19" s="26"/>
       <c r="BC19" s="26"/>
       <c r="BD19" s="26"/>
       <c r="BE19" s="26"/>
-      <c r="BF19" s="27"/>
+      <c r="BF19" s="26"/>
       <c r="BG19" s="27"/>
       <c r="BH19" s="27"/>
       <c r="BI19" s="27"/>
       <c r="BJ19" s="27"/>
-      <c r="BK19" s="26"/>
+      <c r="BK19" s="27"/>
       <c r="BL19" s="26"/>
       <c r="BM19" s="26"/>
       <c r="BN19" s="26"/>
-      <c r="BO19" s="28"/>
-    </row>
-    <row r="20" spans="1:67" ht="15">
+      <c r="BO19" s="26"/>
+      <c r="BP19" s="28"/>
+    </row>
+    <row r="20" spans="1:68" ht="15">
       <c r="B20" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="37">
+        <v>23</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="37">
         <v>43529</v>
       </c>
-      <c r="D20" s="37">
+      <c r="E20" s="37">
         <v>43552</v>
       </c>
-      <c r="E20" s="21">
+      <c r="F20" s="21">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="40">
+      <c r="G20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="40">
         <v>0</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
-      <c r="M20" s="26"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="26"/>
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
       <c r="Q20" s="26"/>
-      <c r="R20" s="25"/>
+      <c r="R20" s="26"/>
       <c r="S20" s="25"/>
-      <c r="T20" s="25"/>
-      <c r="U20" s="25"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="27"/>
-      <c r="AD20" s="27"/>
-      <c r="AE20" s="27"/>
-      <c r="AF20" s="27"/>
-      <c r="AG20" s="26"/>
-      <c r="AH20" s="26"/>
-      <c r="AI20" s="26"/>
-      <c r="AJ20" s="26"/>
-      <c r="AK20" s="26"/>
-      <c r="AL20" s="27"/>
+      <c r="T20" s="66"/>
+      <c r="U20" s="66"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="66"/>
+      <c r="X20" s="82"/>
+      <c r="Y20" s="82"/>
+      <c r="Z20" s="82"/>
+      <c r="AA20" s="82"/>
+      <c r="AB20" s="82"/>
+      <c r="AC20" s="85"/>
+      <c r="AD20" s="85"/>
+      <c r="AE20" s="85"/>
+      <c r="AF20" s="85"/>
+      <c r="AG20" s="85"/>
+      <c r="AH20" s="82"/>
+      <c r="AI20" s="82"/>
+      <c r="AJ20" s="82"/>
+      <c r="AK20" s="82"/>
+      <c r="AL20" s="26"/>
       <c r="AM20" s="27"/>
       <c r="AN20" s="27"/>
       <c r="AO20" s="27"/>
       <c r="AP20" s="27"/>
-      <c r="AQ20" s="26"/>
+      <c r="AQ20" s="27"/>
       <c r="AR20" s="26"/>
       <c r="AS20" s="26"/>
       <c r="AT20" s="26"/>
       <c r="AU20" s="26"/>
-      <c r="AV20" s="25"/>
+      <c r="AV20" s="26"/>
       <c r="AW20" s="25"/>
       <c r="AX20" s="25"/>
       <c r="AY20" s="25"/>
       <c r="AZ20" s="25"/>
-      <c r="BA20" s="26"/>
+      <c r="BA20" s="25"/>
       <c r="BB20" s="26"/>
       <c r="BC20" s="26"/>
       <c r="BD20" s="26"/>
       <c r="BE20" s="26"/>
-      <c r="BF20" s="27"/>
+      <c r="BF20" s="26"/>
       <c r="BG20" s="27"/>
       <c r="BH20" s="27"/>
       <c r="BI20" s="27"/>
       <c r="BJ20" s="27"/>
-      <c r="BK20" s="26"/>
+      <c r="BK20" s="27"/>
       <c r="BL20" s="26"/>
       <c r="BM20" s="26"/>
       <c r="BN20" s="26"/>
-      <c r="BO20" s="28"/>
-    </row>
-    <row r="21" spans="1:67" ht="15">
+      <c r="BO20" s="26"/>
+      <c r="BP20" s="28"/>
+    </row>
+    <row r="21" spans="1:68" ht="15">
       <c r="B21" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="37">
+        <v>32</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="37">
         <v>43531</v>
       </c>
-      <c r="D21" s="37">
+      <c r="E21" s="37">
         <v>43534</v>
       </c>
-      <c r="E21" s="21">
+      <c r="F21" s="21">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="40">
+      <c r="G21" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="40">
         <v>0</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="25"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
-      <c r="M21" s="26"/>
+      <c r="M21" s="25"/>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
-      <c r="R21" s="25"/>
+      <c r="R21" s="26"/>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="26"/>
+      <c r="V21" s="66"/>
+      <c r="W21" s="66"/>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
       <c r="Z21" s="26"/>
       <c r="AA21" s="26"/>
-      <c r="AB21" s="27"/>
+      <c r="AB21" s="26"/>
       <c r="AC21" s="27"/>
       <c r="AD21" s="27"/>
       <c r="AE21" s="27"/>
       <c r="AF21" s="27"/>
-      <c r="AG21" s="26"/>
+      <c r="AG21" s="27"/>
       <c r="AH21" s="26"/>
       <c r="AI21" s="26"/>
       <c r="AJ21" s="26"/>
       <c r="AK21" s="26"/>
-      <c r="AL21" s="27"/>
+      <c r="AL21" s="26"/>
       <c r="AM21" s="27"/>
       <c r="AN21" s="27"/>
       <c r="AO21" s="27"/>
       <c r="AP21" s="27"/>
-      <c r="AQ21" s="26"/>
+      <c r="AQ21" s="27"/>
       <c r="AR21" s="26"/>
       <c r="AS21" s="26"/>
       <c r="AT21" s="26"/>
       <c r="AU21" s="26"/>
-      <c r="AV21" s="25"/>
+      <c r="AV21" s="26"/>
       <c r="AW21" s="25"/>
       <c r="AX21" s="25"/>
       <c r="AY21" s="25"/>
       <c r="AZ21" s="25"/>
-      <c r="BA21" s="26"/>
+      <c r="BA21" s="25"/>
       <c r="BB21" s="26"/>
       <c r="BC21" s="26"/>
       <c r="BD21" s="26"/>
       <c r="BE21" s="26"/>
-      <c r="BF21" s="27"/>
+      <c r="BF21" s="26"/>
       <c r="BG21" s="27"/>
       <c r="BH21" s="27"/>
       <c r="BI21" s="27"/>
       <c r="BJ21" s="27"/>
-      <c r="BK21" s="26"/>
+      <c r="BK21" s="27"/>
       <c r="BL21" s="26"/>
       <c r="BM21" s="26"/>
       <c r="BN21" s="26"/>
-      <c r="BO21" s="28"/>
-    </row>
-    <row r="22" spans="1:67">
+      <c r="BO21" s="26"/>
+      <c r="BP21" s="28"/>
+    </row>
+    <row r="22" spans="1:68">
       <c r="A22" s="14" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B22" s="33"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="36"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="35"/>
       <c r="K22" s="36"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="41"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="34"/>
       <c r="N22" s="41"/>
       <c r="O22" s="41"/>
       <c r="P22" s="41"/>
       <c r="Q22" s="41"/>
-      <c r="R22" s="34"/>
+      <c r="R22" s="41"/>
       <c r="S22" s="34"/>
       <c r="T22" s="34"/>
       <c r="U22" s="34"/>
@@ -2804,490 +2883,509 @@
       <c r="BM22" s="34"/>
       <c r="BN22" s="34"/>
       <c r="BO22" s="34"/>
-    </row>
-    <row r="23" spans="1:67" ht="15">
+      <c r="BP22" s="34"/>
+    </row>
+    <row r="23" spans="1:68" ht="15">
       <c r="B23" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="37">
+        <v>52</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="37">
         <v>43531</v>
       </c>
-      <c r="D23" s="37">
+      <c r="E23" s="37">
         <v>43536</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="40">
+      <c r="F23" s="21"/>
+      <c r="G23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="40">
         <v>0</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="25"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
-      <c r="M23" s="26"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
-      <c r="R23" s="25"/>
+      <c r="R23" s="26"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="82"/>
+      <c r="Y23" s="82"/>
       <c r="Z23" s="26"/>
       <c r="AA23" s="26"/>
-      <c r="AB23" s="27"/>
+      <c r="AB23" s="26"/>
       <c r="AC23" s="27"/>
       <c r="AD23" s="27"/>
       <c r="AE23" s="27"/>
       <c r="AF23" s="27"/>
-      <c r="AG23" s="26"/>
+      <c r="AG23" s="27"/>
       <c r="AH23" s="26"/>
       <c r="AI23" s="26"/>
       <c r="AJ23" s="26"/>
       <c r="AK23" s="26"/>
-      <c r="AL23" s="27"/>
+      <c r="AL23" s="26"/>
       <c r="AM23" s="27"/>
       <c r="AN23" s="27"/>
       <c r="AO23" s="27"/>
       <c r="AP23" s="27"/>
-      <c r="AQ23" s="26"/>
+      <c r="AQ23" s="27"/>
       <c r="AR23" s="26"/>
       <c r="AS23" s="26"/>
       <c r="AT23" s="26"/>
       <c r="AU23" s="26"/>
-      <c r="AV23" s="25"/>
+      <c r="AV23" s="26"/>
       <c r="AW23" s="25"/>
       <c r="AX23" s="25"/>
       <c r="AY23" s="25"/>
       <c r="AZ23" s="25"/>
-      <c r="BA23" s="26"/>
+      <c r="BA23" s="25"/>
       <c r="BB23" s="26"/>
       <c r="BC23" s="26"/>
       <c r="BD23" s="26"/>
       <c r="BE23" s="26"/>
-      <c r="BF23" s="27"/>
+      <c r="BF23" s="26"/>
       <c r="BG23" s="27"/>
       <c r="BH23" s="27"/>
       <c r="BI23" s="27"/>
       <c r="BJ23" s="27"/>
-      <c r="BK23" s="26"/>
+      <c r="BK23" s="27"/>
       <c r="BL23" s="26"/>
       <c r="BM23" s="26"/>
       <c r="BN23" s="26"/>
-      <c r="BO23" s="28"/>
-    </row>
-    <row r="24" spans="1:67" ht="15">
+      <c r="BO23" s="26"/>
+      <c r="BP23" s="28"/>
+    </row>
+    <row r="24" spans="1:68" ht="15">
       <c r="B24" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="37">
+        <v>53</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="37">
         <v>43531</v>
       </c>
-      <c r="D24" s="37">
+      <c r="E24" s="37">
         <v>43536</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="40">
+      <c r="F24" s="21"/>
+      <c r="G24" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="40">
         <v>0</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
       <c r="K24" s="25"/>
       <c r="L24" s="25"/>
-      <c r="M24" s="26"/>
+      <c r="M24" s="25"/>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
-      <c r="R24" s="25"/>
+      <c r="R24" s="26"/>
       <c r="S24" s="25"/>
       <c r="T24" s="25"/>
       <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="66"/>
+      <c r="X24" s="82"/>
+      <c r="Y24" s="82"/>
       <c r="Z24" s="26"/>
       <c r="AA24" s="26"/>
-      <c r="AB24" s="27"/>
+      <c r="AB24" s="26"/>
       <c r="AC24" s="27"/>
       <c r="AD24" s="27"/>
       <c r="AE24" s="27"/>
       <c r="AF24" s="27"/>
-      <c r="AG24" s="26"/>
+      <c r="AG24" s="27"/>
       <c r="AH24" s="26"/>
       <c r="AI24" s="26"/>
       <c r="AJ24" s="26"/>
       <c r="AK24" s="26"/>
-      <c r="AL24" s="27"/>
+      <c r="AL24" s="26"/>
       <c r="AM24" s="27"/>
       <c r="AN24" s="27"/>
       <c r="AO24" s="27"/>
       <c r="AP24" s="27"/>
-      <c r="AQ24" s="26"/>
+      <c r="AQ24" s="27"/>
       <c r="AR24" s="26"/>
       <c r="AS24" s="26"/>
       <c r="AT24" s="26"/>
       <c r="AU24" s="26"/>
-      <c r="AV24" s="25"/>
+      <c r="AV24" s="26"/>
       <c r="AW24" s="25"/>
       <c r="AX24" s="25"/>
       <c r="AY24" s="25"/>
       <c r="AZ24" s="25"/>
-      <c r="BA24" s="26"/>
+      <c r="BA24" s="25"/>
       <c r="BB24" s="26"/>
       <c r="BC24" s="26"/>
       <c r="BD24" s="26"/>
       <c r="BE24" s="26"/>
-      <c r="BF24" s="27"/>
+      <c r="BF24" s="26"/>
       <c r="BG24" s="27"/>
       <c r="BH24" s="27"/>
       <c r="BI24" s="27"/>
       <c r="BJ24" s="27"/>
-      <c r="BK24" s="26"/>
+      <c r="BK24" s="27"/>
       <c r="BL24" s="26"/>
       <c r="BM24" s="26"/>
       <c r="BN24" s="26"/>
-      <c r="BO24" s="28"/>
-    </row>
-    <row r="25" spans="1:67" ht="15">
+      <c r="BO24" s="26"/>
+      <c r="BP24" s="28"/>
+    </row>
+    <row r="25" spans="1:68" ht="15">
       <c r="B25" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="37">
+        <v>41</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="37">
         <v>43531</v>
       </c>
-      <c r="D25" s="37">
+      <c r="E25" s="37">
         <v>43536</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="40">
+      <c r="F25" s="21"/>
+      <c r="G25" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="40">
         <v>0</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="25"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="26"/>
+      <c r="M25" s="25"/>
       <c r="N25" s="26"/>
       <c r="O25" s="26"/>
       <c r="P25" s="26"/>
       <c r="Q25" s="26"/>
-      <c r="R25" s="25"/>
+      <c r="R25" s="26"/>
       <c r="S25" s="25"/>
       <c r="T25" s="25"/>
       <c r="U25" s="25"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
+      <c r="V25" s="66"/>
+      <c r="W25" s="66"/>
+      <c r="X25" s="82"/>
+      <c r="Y25" s="82"/>
       <c r="Z25" s="26"/>
       <c r="AA25" s="26"/>
-      <c r="AB25" s="27"/>
+      <c r="AB25" s="26"/>
       <c r="AC25" s="27"/>
       <c r="AD25" s="27"/>
       <c r="AE25" s="27"/>
       <c r="AF25" s="27"/>
-      <c r="AG25" s="26"/>
+      <c r="AG25" s="27"/>
       <c r="AH25" s="26"/>
       <c r="AI25" s="26"/>
       <c r="AJ25" s="26"/>
       <c r="AK25" s="26"/>
-      <c r="AL25" s="27"/>
+      <c r="AL25" s="26"/>
       <c r="AM25" s="27"/>
       <c r="AN25" s="27"/>
       <c r="AO25" s="27"/>
       <c r="AP25" s="27"/>
-      <c r="AQ25" s="26"/>
+      <c r="AQ25" s="27"/>
       <c r="AR25" s="26"/>
       <c r="AS25" s="26"/>
       <c r="AT25" s="26"/>
       <c r="AU25" s="26"/>
-      <c r="AV25" s="25"/>
+      <c r="AV25" s="26"/>
       <c r="AW25" s="25"/>
       <c r="AX25" s="25"/>
       <c r="AY25" s="25"/>
       <c r="AZ25" s="25"/>
-      <c r="BA25" s="26"/>
+      <c r="BA25" s="25"/>
       <c r="BB25" s="26"/>
       <c r="BC25" s="26"/>
       <c r="BD25" s="26"/>
       <c r="BE25" s="26"/>
-      <c r="BF25" s="27"/>
+      <c r="BF25" s="26"/>
       <c r="BG25" s="27"/>
       <c r="BH25" s="27"/>
       <c r="BI25" s="27"/>
       <c r="BJ25" s="27"/>
-      <c r="BK25" s="26"/>
+      <c r="BK25" s="27"/>
       <c r="BL25" s="26"/>
       <c r="BM25" s="26"/>
       <c r="BN25" s="26"/>
-      <c r="BO25" s="28"/>
-    </row>
-    <row r="26" spans="1:67" ht="15">
+      <c r="BO25" s="26"/>
+      <c r="BP25" s="28"/>
+    </row>
+    <row r="26" spans="1:68" ht="15">
       <c r="B26" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="37">
+        <v>40</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="37">
         <v>43538</v>
       </c>
-      <c r="D26" s="37">
+      <c r="E26" s="37">
         <v>43545</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="40">
+      <c r="F26" s="21"/>
+      <c r="G26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="40">
         <v>0</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="25"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="25"/>
       <c r="L26" s="25"/>
-      <c r="M26" s="26"/>
+      <c r="M26" s="25"/>
       <c r="N26" s="26"/>
       <c r="O26" s="26"/>
       <c r="P26" s="26"/>
       <c r="Q26" s="26"/>
-      <c r="R26" s="25"/>
+      <c r="R26" s="26"/>
       <c r="S26" s="25"/>
       <c r="T26" s="25"/>
       <c r="U26" s="25"/>
       <c r="V26" s="25"/>
-      <c r="W26" s="26"/>
+      <c r="W26" s="25"/>
       <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="27"/>
-      <c r="AC26" s="27"/>
-      <c r="AD26" s="27"/>
-      <c r="AE26" s="27"/>
-      <c r="AF26" s="27"/>
-      <c r="AG26" s="26"/>
+      <c r="AA26" s="82"/>
+      <c r="AB26" s="82"/>
+      <c r="AC26" s="85"/>
+      <c r="AD26" s="85"/>
+      <c r="AE26" s="85"/>
+      <c r="AF26" s="85"/>
+      <c r="AG26" s="27"/>
       <c r="AH26" s="26"/>
       <c r="AI26" s="26"/>
       <c r="AJ26" s="26"/>
       <c r="AK26" s="26"/>
-      <c r="AL26" s="27"/>
+      <c r="AL26" s="26"/>
       <c r="AM26" s="27"/>
       <c r="AN26" s="27"/>
       <c r="AO26" s="27"/>
       <c r="AP26" s="27"/>
-      <c r="AQ26" s="26"/>
+      <c r="AQ26" s="27"/>
       <c r="AR26" s="26"/>
       <c r="AS26" s="26"/>
       <c r="AT26" s="26"/>
       <c r="AU26" s="26"/>
-      <c r="AV26" s="25"/>
+      <c r="AV26" s="26"/>
       <c r="AW26" s="25"/>
       <c r="AX26" s="25"/>
       <c r="AY26" s="25"/>
       <c r="AZ26" s="25"/>
-      <c r="BA26" s="26"/>
+      <c r="BA26" s="25"/>
       <c r="BB26" s="26"/>
       <c r="BC26" s="26"/>
       <c r="BD26" s="26"/>
       <c r="BE26" s="26"/>
-      <c r="BF26" s="27"/>
+      <c r="BF26" s="26"/>
       <c r="BG26" s="27"/>
       <c r="BH26" s="27"/>
       <c r="BI26" s="27"/>
       <c r="BJ26" s="27"/>
-      <c r="BK26" s="26"/>
+      <c r="BK26" s="27"/>
       <c r="BL26" s="26"/>
       <c r="BM26" s="26"/>
       <c r="BN26" s="26"/>
-      <c r="BO26" s="28"/>
-    </row>
-    <row r="27" spans="1:67" ht="15">
+      <c r="BO26" s="26"/>
+      <c r="BP26" s="28"/>
+    </row>
+    <row r="27" spans="1:68" ht="15">
       <c r="B27" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="37">
+        <v>42</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="37">
         <v>43545</v>
       </c>
-      <c r="D27" s="37">
+      <c r="E27" s="37">
         <v>43552</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="40">
+      <c r="F27" s="21"/>
+      <c r="G27" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="40">
         <v>0</v>
       </c>
-      <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="25"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="24"/>
       <c r="K27" s="25"/>
       <c r="L27" s="25"/>
-      <c r="M27" s="26"/>
+      <c r="M27" s="25"/>
       <c r="N27" s="26"/>
       <c r="O27" s="26"/>
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
-      <c r="R27" s="25"/>
+      <c r="R27" s="26"/>
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
+      <c r="W27" s="25"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26"/>
       <c r="Z27" s="26"/>
       <c r="AA27" s="26"/>
-      <c r="AB27" s="27"/>
+      <c r="AB27" s="26"/>
       <c r="AC27" s="27"/>
       <c r="AD27" s="27"/>
       <c r="AE27" s="27"/>
-      <c r="AF27" s="27"/>
-      <c r="AG27" s="26"/>
-      <c r="AH27" s="26"/>
-      <c r="AI27" s="26"/>
-      <c r="AJ27" s="26"/>
-      <c r="AK27" s="26"/>
-      <c r="AL27" s="27"/>
+      <c r="AF27" s="85"/>
+      <c r="AG27" s="85"/>
+      <c r="AH27" s="82"/>
+      <c r="AI27" s="82"/>
+      <c r="AJ27" s="82"/>
+      <c r="AK27" s="82"/>
+      <c r="AL27" s="26"/>
       <c r="AM27" s="27"/>
       <c r="AN27" s="27"/>
       <c r="AO27" s="27"/>
       <c r="AP27" s="27"/>
-      <c r="AQ27" s="26"/>
+      <c r="AQ27" s="27"/>
       <c r="AR27" s="26"/>
       <c r="AS27" s="26"/>
       <c r="AT27" s="26"/>
       <c r="AU27" s="26"/>
-      <c r="AV27" s="25"/>
+      <c r="AV27" s="26"/>
       <c r="AW27" s="25"/>
       <c r="AX27" s="25"/>
       <c r="AY27" s="25"/>
       <c r="AZ27" s="25"/>
-      <c r="BA27" s="26"/>
+      <c r="BA27" s="25"/>
       <c r="BB27" s="26"/>
       <c r="BC27" s="26"/>
       <c r="BD27" s="26"/>
       <c r="BE27" s="26"/>
-      <c r="BF27" s="27"/>
+      <c r="BF27" s="26"/>
       <c r="BG27" s="27"/>
       <c r="BH27" s="27"/>
       <c r="BI27" s="27"/>
       <c r="BJ27" s="27"/>
-      <c r="BK27" s="26"/>
+      <c r="BK27" s="27"/>
       <c r="BL27" s="26"/>
       <c r="BM27" s="26"/>
       <c r="BN27" s="26"/>
-      <c r="BO27" s="28"/>
-    </row>
-    <row r="28" spans="1:67" ht="15">
+      <c r="BO27" s="26"/>
+      <c r="BP27" s="28"/>
+    </row>
+    <row r="28" spans="1:68" ht="15">
       <c r="B28" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="37">
+        <v>43552</v>
+      </c>
+      <c r="E28" s="37">
+        <v>43554</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="37">
-        <v>43552</v>
-      </c>
-      <c r="D28" s="37">
-        <v>43554</v>
-      </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="40">
+      <c r="H28" s="40">
         <v>0</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="24"/>
       <c r="K28" s="25"/>
       <c r="L28" s="25"/>
-      <c r="M28" s="26"/>
+      <c r="M28" s="25"/>
       <c r="N28" s="26"/>
       <c r="O28" s="26"/>
       <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
-      <c r="R28" s="25"/>
+      <c r="R28" s="26"/>
       <c r="S28" s="25"/>
       <c r="T28" s="25"/>
       <c r="U28" s="25"/>
       <c r="V28" s="25"/>
-      <c r="W28" s="26"/>
+      <c r="W28" s="25"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
       <c r="Z28" s="26"/>
       <c r="AA28" s="26"/>
-      <c r="AB28" s="27"/>
+      <c r="AB28" s="26"/>
       <c r="AC28" s="27"/>
       <c r="AD28" s="27"/>
       <c r="AE28" s="27"/>
       <c r="AF28" s="27"/>
-      <c r="AG28" s="26"/>
+      <c r="AG28" s="27"/>
       <c r="AH28" s="26"/>
       <c r="AI28" s="26"/>
       <c r="AJ28" s="26"/>
-      <c r="AK28" s="26"/>
-      <c r="AL28" s="27"/>
+      <c r="AK28" s="82"/>
+      <c r="AL28" s="82"/>
       <c r="AM28" s="27"/>
       <c r="AN28" s="27"/>
       <c r="AO28" s="27"/>
       <c r="AP28" s="27"/>
-      <c r="AQ28" s="26"/>
+      <c r="AQ28" s="27"/>
       <c r="AR28" s="26"/>
       <c r="AS28" s="26"/>
       <c r="AT28" s="26"/>
       <c r="AU28" s="26"/>
-      <c r="AV28" s="25"/>
+      <c r="AV28" s="26"/>
       <c r="AW28" s="25"/>
       <c r="AX28" s="25"/>
       <c r="AY28" s="25"/>
       <c r="AZ28" s="25"/>
-      <c r="BA28" s="26"/>
+      <c r="BA28" s="25"/>
       <c r="BB28" s="26"/>
       <c r="BC28" s="26"/>
       <c r="BD28" s="26"/>
       <c r="BE28" s="26"/>
-      <c r="BF28" s="27"/>
+      <c r="BF28" s="26"/>
       <c r="BG28" s="27"/>
       <c r="BH28" s="27"/>
       <c r="BI28" s="27"/>
       <c r="BJ28" s="27"/>
-      <c r="BK28" s="26"/>
+      <c r="BK28" s="27"/>
       <c r="BL28" s="26"/>
       <c r="BM28" s="26"/>
       <c r="BN28" s="26"/>
-      <c r="BO28" s="28"/>
-    </row>
-    <row r="29" spans="1:67">
+      <c r="BO28" s="26"/>
+      <c r="BP28" s="28"/>
+    </row>
+    <row r="29" spans="1:68">
       <c r="A29" s="14" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B29" s="33"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="36"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="35"/>
       <c r="K29" s="36"/>
-      <c r="L29" s="34"/>
+      <c r="L29" s="36"/>
       <c r="M29" s="34"/>
       <c r="N29" s="34"/>
       <c r="O29" s="34"/>
@@ -3343,320 +3441,333 @@
       <c r="BM29" s="34"/>
       <c r="BN29" s="34"/>
       <c r="BO29" s="34"/>
-    </row>
-    <row r="30" spans="1:67" ht="15">
+      <c r="BP29" s="34"/>
+    </row>
+    <row r="30" spans="1:68" ht="15">
       <c r="B30" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="37">
+        <v>44</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="37">
         <v>43557</v>
       </c>
-      <c r="D30" s="37">
+      <c r="E30" s="37">
         <v>43560</v>
       </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="40">
+      <c r="F30" s="21"/>
+      <c r="G30" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="40">
         <v>0</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="25"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
       <c r="K30" s="25"/>
       <c r="L30" s="25"/>
-      <c r="M30" s="26"/>
+      <c r="M30" s="25"/>
       <c r="N30" s="26"/>
       <c r="O30" s="26"/>
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
-      <c r="R30" s="25"/>
+      <c r="R30" s="26"/>
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
       <c r="U30" s="25"/>
       <c r="V30" s="25"/>
-      <c r="W30" s="26"/>
+      <c r="W30" s="25"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
       <c r="Z30" s="26"/>
       <c r="AA30" s="26"/>
-      <c r="AB30" s="27"/>
+      <c r="AB30" s="26"/>
       <c r="AC30" s="27"/>
       <c r="AD30" s="27"/>
       <c r="AE30" s="27"/>
       <c r="AF30" s="27"/>
-      <c r="AG30" s="26"/>
+      <c r="AG30" s="27"/>
       <c r="AH30" s="26"/>
       <c r="AI30" s="26"/>
       <c r="AJ30" s="26"/>
       <c r="AK30" s="26"/>
-      <c r="AL30" s="27"/>
+      <c r="AL30" s="26"/>
       <c r="AM30" s="27"/>
-      <c r="AN30" s="27"/>
-      <c r="AO30" s="27"/>
-      <c r="AP30" s="27"/>
-      <c r="AQ30" s="26"/>
+      <c r="AN30" s="85"/>
+      <c r="AO30" s="85"/>
+      <c r="AP30" s="85"/>
+      <c r="AQ30" s="85"/>
       <c r="AR30" s="26"/>
       <c r="AS30" s="26"/>
       <c r="AT30" s="26"/>
       <c r="AU30" s="26"/>
-      <c r="AV30" s="25"/>
+      <c r="AV30" s="26"/>
       <c r="AW30" s="25"/>
       <c r="AX30" s="25"/>
       <c r="AY30" s="25"/>
       <c r="AZ30" s="25"/>
-      <c r="BA30" s="26"/>
+      <c r="BA30" s="25"/>
       <c r="BB30" s="26"/>
       <c r="BC30" s="26"/>
       <c r="BD30" s="26"/>
       <c r="BE30" s="26"/>
-      <c r="BF30" s="27"/>
+      <c r="BF30" s="26"/>
       <c r="BG30" s="27"/>
       <c r="BH30" s="27"/>
       <c r="BI30" s="27"/>
       <c r="BJ30" s="27"/>
-      <c r="BK30" s="26"/>
+      <c r="BK30" s="27"/>
       <c r="BL30" s="26"/>
       <c r="BM30" s="26"/>
       <c r="BN30" s="26"/>
-      <c r="BO30" s="28"/>
-    </row>
-    <row r="31" spans="1:67" s="45" customFormat="1" ht="15">
+      <c r="BO30" s="26"/>
+      <c r="BP30" s="28"/>
+    </row>
+    <row r="31" spans="1:68" s="45" customFormat="1" ht="15">
       <c r="B31" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="37">
+        <v>47</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="37">
         <v>43560</v>
       </c>
-      <c r="D31" s="37">
+      <c r="E31" s="37">
         <v>43572</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" s="40">
+      <c r="F31" s="21"/>
+      <c r="G31" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="40">
         <v>0</v>
       </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="25"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="24"/>
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
-      <c r="M31" s="26"/>
+      <c r="M31" s="25"/>
       <c r="N31" s="26"/>
       <c r="O31" s="26"/>
       <c r="P31" s="26"/>
       <c r="Q31" s="26"/>
-      <c r="R31" s="25"/>
+      <c r="R31" s="26"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25"/>
       <c r="V31" s="25"/>
-      <c r="W31" s="26"/>
+      <c r="W31" s="25"/>
       <c r="X31" s="26"/>
       <c r="Y31" s="26"/>
       <c r="Z31" s="26"/>
       <c r="AA31" s="26"/>
-      <c r="AB31" s="27"/>
+      <c r="AB31" s="26"/>
       <c r="AC31" s="27"/>
       <c r="AD31" s="27"/>
       <c r="AE31" s="27"/>
       <c r="AF31" s="27"/>
-      <c r="AG31" s="26"/>
+      <c r="AG31" s="27"/>
       <c r="AH31" s="26"/>
       <c r="AI31" s="26"/>
       <c r="AJ31" s="26"/>
       <c r="AK31" s="26"/>
-      <c r="AL31" s="27"/>
+      <c r="AL31" s="26"/>
       <c r="AM31" s="27"/>
       <c r="AN31" s="27"/>
       <c r="AO31" s="27"/>
       <c r="AP31" s="27"/>
-      <c r="AQ31" s="26"/>
-      <c r="AR31" s="26"/>
-      <c r="AS31" s="26"/>
-      <c r="AT31" s="26"/>
-      <c r="AU31" s="26"/>
-      <c r="AV31" s="25"/>
-      <c r="AW31" s="25"/>
-      <c r="AX31" s="25"/>
-      <c r="AY31" s="25"/>
+      <c r="AQ31" s="85"/>
+      <c r="AR31" s="82"/>
+      <c r="AS31" s="82"/>
+      <c r="AT31" s="82"/>
+      <c r="AU31" s="82"/>
+      <c r="AV31" s="82"/>
+      <c r="AW31" s="66"/>
+      <c r="AX31" s="66"/>
+      <c r="AY31" s="66"/>
       <c r="AZ31" s="25"/>
-      <c r="BA31" s="26"/>
+      <c r="BA31" s="25"/>
       <c r="BB31" s="26"/>
       <c r="BC31" s="26"/>
       <c r="BD31" s="26"/>
       <c r="BE31" s="26"/>
-      <c r="BF31" s="27"/>
+      <c r="BF31" s="26"/>
       <c r="BG31" s="27"/>
       <c r="BH31" s="27"/>
       <c r="BI31" s="27"/>
       <c r="BJ31" s="27"/>
-      <c r="BK31" s="26"/>
+      <c r="BK31" s="27"/>
       <c r="BL31" s="26"/>
       <c r="BM31" s="26"/>
       <c r="BN31" s="26"/>
-      <c r="BO31" s="28"/>
-    </row>
-    <row r="32" spans="1:67" ht="15">
+      <c r="BO31" s="26"/>
+      <c r="BP31" s="28"/>
+    </row>
+    <row r="32" spans="1:68" ht="15">
       <c r="B32" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="37">
+        <v>39</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="37">
         <v>43563</v>
       </c>
-      <c r="D32" s="37">
+      <c r="E32" s="37">
         <v>43567</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="40">
+      <c r="F32" s="21"/>
+      <c r="G32" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="40">
         <v>0</v>
       </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="25"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="24"/>
       <c r="K32" s="25"/>
       <c r="L32" s="25"/>
-      <c r="M32" s="26"/>
+      <c r="M32" s="25"/>
       <c r="N32" s="26"/>
       <c r="O32" s="26"/>
       <c r="P32" s="26"/>
       <c r="Q32" s="26"/>
-      <c r="R32" s="25"/>
+      <c r="R32" s="26"/>
       <c r="S32" s="25"/>
       <c r="T32" s="25"/>
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
-      <c r="W32" s="26"/>
+      <c r="W32" s="25"/>
       <c r="X32" s="26"/>
       <c r="Y32" s="26"/>
       <c r="Z32" s="26"/>
       <c r="AA32" s="26"/>
-      <c r="AB32" s="27"/>
+      <c r="AB32" s="26"/>
       <c r="AC32" s="27"/>
       <c r="AD32" s="27"/>
       <c r="AE32" s="27"/>
       <c r="AF32" s="27"/>
-      <c r="AG32" s="26"/>
+      <c r="AG32" s="27"/>
       <c r="AH32" s="26"/>
       <c r="AI32" s="26"/>
       <c r="AJ32" s="26"/>
       <c r="AK32" s="26"/>
-      <c r="AL32" s="27"/>
+      <c r="AL32" s="26"/>
       <c r="AM32" s="27"/>
       <c r="AN32" s="27"/>
       <c r="AO32" s="27"/>
       <c r="AP32" s="27"/>
-      <c r="AQ32" s="26"/>
-      <c r="AR32" s="26"/>
-      <c r="AS32" s="26"/>
-      <c r="AT32" s="26"/>
-      <c r="AU32" s="26"/>
-      <c r="AV32" s="25"/>
+      <c r="AQ32" s="27"/>
+      <c r="AR32" s="82"/>
+      <c r="AS32" s="82"/>
+      <c r="AT32" s="82"/>
+      <c r="AU32" s="82"/>
+      <c r="AV32" s="82"/>
       <c r="AW32" s="25"/>
       <c r="AX32" s="25"/>
       <c r="AY32" s="25"/>
       <c r="AZ32" s="25"/>
-      <c r="BA32" s="26"/>
+      <c r="BA32" s="25"/>
       <c r="BB32" s="26"/>
       <c r="BC32" s="26"/>
       <c r="BD32" s="26"/>
       <c r="BE32" s="26"/>
-      <c r="BF32" s="27"/>
+      <c r="BF32" s="26"/>
       <c r="BG32" s="27"/>
       <c r="BH32" s="27"/>
       <c r="BI32" s="27"/>
       <c r="BJ32" s="27"/>
-      <c r="BK32" s="26"/>
+      <c r="BK32" s="27"/>
       <c r="BL32" s="26"/>
       <c r="BM32" s="26"/>
       <c r="BN32" s="26"/>
-      <c r="BO32" s="28"/>
-    </row>
-    <row r="33" spans="1:67" ht="15">
+      <c r="BO32" s="26"/>
+      <c r="BP32" s="28"/>
+    </row>
+    <row r="33" spans="1:68" ht="15">
       <c r="B33" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="37">
+        <v>46</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="37">
         <v>43567</v>
       </c>
-      <c r="D33" s="37">
+      <c r="E33" s="37">
         <v>43569</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="40">
+      <c r="F33" s="21"/>
+      <c r="G33" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="40">
         <v>0</v>
       </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="25"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="24"/>
       <c r="K33" s="25"/>
       <c r="L33" s="25"/>
-      <c r="M33" s="26"/>
+      <c r="M33" s="25"/>
       <c r="N33" s="26"/>
       <c r="O33" s="26"/>
       <c r="P33" s="26"/>
       <c r="Q33" s="26"/>
-      <c r="R33" s="25"/>
+      <c r="R33" s="26"/>
       <c r="S33" s="25"/>
       <c r="T33" s="25"/>
       <c r="U33" s="25"/>
       <c r="V33" s="25"/>
-      <c r="W33" s="26"/>
+      <c r="W33" s="25"/>
       <c r="X33" s="26"/>
       <c r="Y33" s="26"/>
       <c r="Z33" s="26"/>
       <c r="AA33" s="26"/>
-      <c r="AB33" s="27"/>
+      <c r="AB33" s="26"/>
       <c r="AC33" s="27"/>
       <c r="AD33" s="27"/>
       <c r="AE33" s="27"/>
       <c r="AF33" s="27"/>
-      <c r="AG33" s="26"/>
+      <c r="AG33" s="27"/>
       <c r="AH33" s="26"/>
       <c r="AI33" s="26"/>
       <c r="AJ33" s="26"/>
       <c r="AK33" s="26"/>
-      <c r="AL33" s="27"/>
+      <c r="AL33" s="26"/>
       <c r="AM33" s="27"/>
       <c r="AN33" s="27"/>
       <c r="AO33" s="27"/>
       <c r="AP33" s="27"/>
-      <c r="AQ33" s="26"/>
+      <c r="AQ33" s="27"/>
       <c r="AR33" s="26"/>
       <c r="AS33" s="26"/>
       <c r="AT33" s="26"/>
       <c r="AU33" s="26"/>
-      <c r="AV33" s="25"/>
+      <c r="AV33" s="82"/>
       <c r="AW33" s="25"/>
       <c r="AX33" s="25"/>
       <c r="AY33" s="25"/>
       <c r="AZ33" s="25"/>
-      <c r="BA33" s="26"/>
+      <c r="BA33" s="25"/>
       <c r="BB33" s="26"/>
       <c r="BC33" s="26"/>
       <c r="BD33" s="26"/>
       <c r="BE33" s="26"/>
-      <c r="BF33" s="27"/>
+      <c r="BF33" s="26"/>
       <c r="BG33" s="27"/>
       <c r="BH33" s="27"/>
       <c r="BI33" s="27"/>
       <c r="BJ33" s="27"/>
-      <c r="BK33" s="26"/>
+      <c r="BK33" s="27"/>
       <c r="BL33" s="26"/>
       <c r="BM33" s="26"/>
       <c r="BN33" s="26"/>
-      <c r="BO33" s="28"/>
-    </row>
-    <row r="34" spans="1:67" ht="15.75" customHeight="1">
+      <c r="BO33" s="26"/>
+      <c r="BP33" s="28"/>
+    </row>
+    <row r="34" spans="1:68" ht="15.75" customHeight="1">
       <c r="A34" s="42"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3664,8 +3775,9 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:67" ht="15.75" customHeight="1">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:68" ht="15.75" customHeight="1">
       <c r="A35" s="42"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3673,8 +3785,9 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:67" ht="15.75" customHeight="1">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:68" ht="15.75" customHeight="1">
       <c r="A36" s="42"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3682,41 +3795,42 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:67" ht="15.75" customHeight="1">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:68" ht="15.75" customHeight="1">
       <c r="A37" s="43"/>
     </row>
-    <row r="38" spans="1:67" ht="12.75">
+    <row r="38" spans="1:68" ht="12.75">
       <c r="A38" s="43"/>
     </row>
-    <row r="39" spans="1:67" ht="12.75">
+    <row r="39" spans="1:68" ht="12.75">
       <c r="A39" s="43"/>
     </row>
-    <row r="40" spans="1:67" ht="12.75">
+    <row r="40" spans="1:68" ht="12.75">
       <c r="A40" s="43"/>
     </row>
-    <row r="41" spans="1:67" ht="12.75">
+    <row r="41" spans="1:68" ht="12.75">
       <c r="A41" s="43"/>
     </row>
-    <row r="42" spans="1:67" ht="12.75">
+    <row r="42" spans="1:68" ht="12.75">
       <c r="A42" s="43"/>
     </row>
-    <row r="43" spans="1:67" ht="12.75">
+    <row r="43" spans="1:68" ht="12.75">
       <c r="A43" s="43"/>
     </row>
-    <row r="44" spans="1:67" ht="12.75">
+    <row r="44" spans="1:68" ht="12.75">
       <c r="A44" s="43"/>
     </row>
-    <row r="45" spans="1:67" ht="12.75">
+    <row r="45" spans="1:68" ht="12.75">
       <c r="A45" s="43"/>
     </row>
-    <row r="46" spans="1:67" ht="12.75">
+    <row r="46" spans="1:68" ht="12.75">
       <c r="A46" s="43"/>
     </row>
-    <row r="47" spans="1:67" ht="12.75">
+    <row r="47" spans="1:68" ht="12.75">
       <c r="A47" s="43"/>
     </row>
-    <row r="48" spans="1:67" ht="12.75">
+    <row r="48" spans="1:68" ht="12.75">
       <c r="A48" s="43"/>
     </row>
     <row r="49" spans="1:1" ht="12.75">
@@ -6455,51 +6569,50 @@
     <row r="960" spans="1:1" ht="12.75">
       <c r="A960" s="43"/>
     </row>
-    <row r="961" spans="1:67" ht="12.75">
+    <row r="961" spans="1:68" ht="12.75">
       <c r="A961" s="43"/>
     </row>
-    <row r="962" spans="1:67" ht="12.75">
+    <row r="962" spans="1:68" ht="12.75">
       <c r="A962" s="43"/>
     </row>
-    <row r="963" spans="1:67" ht="12.75">
+    <row r="963" spans="1:68" ht="12.75">
       <c r="A963" s="43"/>
     </row>
-    <row r="964" spans="1:67" ht="12.75">
+    <row r="964" spans="1:68" ht="12.75">
       <c r="A964" s="43"/>
     </row>
-    <row r="965" spans="1:67" ht="12.75">
+    <row r="965" spans="1:68" ht="12.75">
       <c r="A965" s="43"/>
     </row>
-    <row r="966" spans="1:67" ht="12.75">
+    <row r="966" spans="1:68" ht="12.75">
       <c r="A966" s="43"/>
     </row>
-    <row r="967" spans="1:67" ht="12.75">
+    <row r="967" spans="1:68" ht="12.75">
       <c r="A967" s="43"/>
     </row>
-    <row r="968" spans="1:67" ht="12.75">
+    <row r="968" spans="1:68" ht="12.75">
       <c r="A968" s="43"/>
     </row>
-    <row r="969" spans="1:67" ht="12.75">
+    <row r="969" spans="1:68" ht="12.75">
       <c r="A969" s="43"/>
     </row>
-    <row r="970" spans="1:67" ht="12.75">
+    <row r="970" spans="1:68" ht="12.75">
       <c r="A970" s="43"/>
     </row>
-    <row r="971" spans="1:67" ht="12.75">
+    <row r="971" spans="1:68" ht="12.75">
       <c r="A971" s="43"/>
     </row>
-    <row r="972" spans="1:67" ht="12.75">
+    <row r="972" spans="1:68" ht="12.75">
       <c r="A972" s="43"/>
     </row>
-    <row r="973" spans="1:67" ht="12.75">
+    <row r="973" spans="1:68" ht="12.75">
       <c r="A973" s="43"/>
     </row>
-    <row r="974" spans="1:67" ht="12.75">
+    <row r="974" spans="1:68" ht="12.75">
       <c r="A974" s="43"/>
     </row>
-    <row r="975" spans="1:67" ht="12.75">
+    <row r="975" spans="1:68" ht="12.75">
       <c r="A975" s="43"/>
-      <c r="H975" s="4"/>
       <c r="I975" s="4"/>
       <c r="J975" s="4"/>
       <c r="K975" s="4"/>
@@ -6559,8 +6672,9 @@
       <c r="BM975" s="4"/>
       <c r="BN975" s="4"/>
       <c r="BO975" s="4"/>
-    </row>
-    <row r="976" spans="1:67" ht="12.75">
+      <c r="BP975" s="4"/>
+    </row>
+    <row r="976" spans="1:68" ht="12.75">
       <c r="A976" s="43"/>
     </row>
     <row r="977" spans="1:1" ht="12.75">
@@ -6611,58 +6725,60 @@
     <row r="992" spans="1:1" ht="12.75">
       <c r="A992" s="43"/>
     </row>
-    <row r="993" spans="1:7" ht="12.75">
+    <row r="993" spans="1:8" ht="12.75">
       <c r="A993" s="43"/>
     </row>
-    <row r="994" spans="1:7" ht="12.75">
+    <row r="994" spans="1:8" ht="12.75">
       <c r="A994" s="43"/>
     </row>
-    <row r="995" spans="1:7" ht="12.75">
+    <row r="995" spans="1:8" ht="12.75">
       <c r="A995" s="43"/>
     </row>
-    <row r="996" spans="1:7" ht="12.75">
+    <row r="996" spans="1:8" ht="12.75">
       <c r="A996" s="43"/>
     </row>
-    <row r="997" spans="1:7" ht="12.75">
+    <row r="997" spans="1:8" ht="12.75">
       <c r="A997" s="43"/>
     </row>
-    <row r="998" spans="1:7" ht="12.75">
+    <row r="998" spans="1:8" ht="12.75">
       <c r="A998" s="44"/>
       <c r="B998" s="4"/>
-      <c r="C998" s="4"/>
+      <c r="C998" s="47"/>
       <c r="D998" s="4"/>
       <c r="E998" s="4"/>
       <c r="F998" s="4"/>
       <c r="G998" s="4"/>
+      <c r="H998" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="BF6:BJ6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="W6:AA6"/>
-    <mergeCell ref="BK6:BO6"/>
+  <mergeCells count="25">
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="BL6:BP6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="AL6:AP6"/>
-    <mergeCell ref="AQ6:AU6"/>
-    <mergeCell ref="AV6:AZ6"/>
-    <mergeCell ref="BA6:BE6"/>
-    <mergeCell ref="AG6:AK6"/>
-    <mergeCell ref="AB6:AF6"/>
-    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="AM6:AQ6"/>
+    <mergeCell ref="AR6:AV6"/>
+    <mergeCell ref="AW6:BA6"/>
+    <mergeCell ref="BB6:BF6"/>
+    <mergeCell ref="AH6:AL6"/>
+    <mergeCell ref="AC6:AG6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="X6:AB6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G17:G21 G9:G15 G23:G28 G30:G33">
+  <conditionalFormatting sqref="H17:H21 H9:H15 H23:H28 H30:H33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="0"/>

</xml_diff>